<commit_message>
Integrated ELL Comparison figures
</commit_message>
<xml_diff>
--- a/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
+++ b/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>SpMV Only</t>
+  </si>
+  <si>
+    <t>Comm Only</t>
   </si>
 </sst>
 </file>
@@ -86,8 +89,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -96,11 +101,13 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -441,7 +448,7 @@
     <col min="4" max="4" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>17</v>
       </c>
@@ -452,7 +459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -465,8 +472,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1</v>
       </c>
@@ -479,47 +492,74 @@
       <c r="D3">
         <v>16.537800000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>16.529499999999999</v>
+      </c>
+      <c r="F3">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4">
+        <v>41.249000000000002</v>
+      </c>
+      <c r="E4">
+        <v>10.4048</v>
+      </c>
+      <c r="F4">
+        <v>26.385000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>42.650300000000001</v>
+      </c>
+      <c r="E5">
+        <v>6.5306199999999999</v>
+      </c>
+      <c r="F5">
+        <v>28.780999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
         <v>22.901499999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>41.249000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>10.1092</v>
+      </c>
+      <c r="F6">
+        <v>6.8635999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>2</v>
       </c>
@@ -532,50 +572,65 @@
       <c r="D7">
         <v>31.880600000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>5.4991500000000002</v>
+      </c>
+      <c r="F7">
+        <v>19.2149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8">
         <v>8</v>
       </c>
       <c r="D8">
-        <v>12.529299999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>16.781400000000001</v>
+      </c>
+      <c r="E8">
+        <v>4.0113000000000003</v>
+      </c>
+      <c r="F8">
+        <v>7.9760499999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
-      <c r="D9">
-        <v>42.650300000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
       <c r="D10">
-        <v>16.781400000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>12.529299999999999</v>
+      </c>
+      <c r="E10">
+        <v>2.54644</v>
+      </c>
+      <c r="F10">
+        <v>6.11653</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>4</v>
       </c>
@@ -588,147 +643,16 @@
       <c r="D11">
         <v>11.052199999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>16.537800000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>22.901499999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16">
-        <v>4</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
-        <v>1</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>41.249000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
-        <v>2</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>4</v>
-      </c>
-      <c r="D18">
-        <v>31.880600000000001</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>12.529299999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>42.650300000000001</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
-        <v>2</v>
-      </c>
-      <c r="B21">
-        <v>4</v>
-      </c>
-      <c r="C21">
-        <v>8</v>
-      </c>
-      <c r="D21">
-        <v>16.781400000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
-        <v>4</v>
-      </c>
-      <c r="B22">
-        <v>4</v>
-      </c>
-      <c r="C22">
-        <v>16</v>
-      </c>
-      <c r="D22">
-        <v>11.052199999999999</v>
+      <c r="E11">
+        <v>1.1715</v>
+      </c>
+      <c r="F11">
+        <v>7.0250500000000002</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:D11">
-    <sortCondition ref="B4"/>
+  <sortState ref="A3:E11">
+    <sortCondition ref="A3"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added a new gflops figure for strong scaling
</commit_message>
<xml_diff>
--- a/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
+++ b/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="3340" windowWidth="33860" windowHeight="28360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26540" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="m2070_nooverlap_vcl" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
   <si>
     <t>Time (ms)</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>nodes</t>
+  </si>
+  <si>
+    <t>SpMV Only</t>
+  </si>
+  <si>
+    <t>Comm Only</t>
+  </si>
+  <si>
+    <t>SpMV + Comm</t>
   </si>
   <si>
     <t>n=17</t>
@@ -92,6 +101,9 @@
   <si>
     <t>Speedup tells how much faster the overlapping solution is compared to the non-overlapping solution</t>
   </si>
+  <si>
+    <t>% of Time Total in Comm</t>
+  </si>
 </sst>
 </file>
 
@@ -100,7 +112,14 @@
   <numFmts count="1">
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -142,378 +161,403 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="369">
+  <cellStyleXfs count="394">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -524,377 +568,403 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="369">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="296" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="306" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="314" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="316" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="318" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="320" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="322" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="324" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="326" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="328" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="330" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="332" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="334" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="336" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="338" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="340" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="342" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="344" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="346" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="348" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="350" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="352" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="354" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="356" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="358" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="360" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="295" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="305" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="313" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="315" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="317" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="319" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="321" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="323" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="325" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="327" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="329" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="331" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="333" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="335" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="337" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="339" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="341" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="343" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="345" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="347" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="349" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="351" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="353" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="355" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="357" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="359" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+  <cellStyles count="394">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="169" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="171" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="211" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="213" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="215" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="217" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="219" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="221" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="223" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="225" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="245" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="247" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="249" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="251" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="253" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="255" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="257" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="259" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="261" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="263" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="265" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="267" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="269" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="271" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="281" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="283" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="285" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="287" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="289" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="291" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="293" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="295" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="309" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="311" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="313" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="343" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="345" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="347" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="349" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="351" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="353" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="355" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="357" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="359" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="361" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="363" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="365" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="367" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="369" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="371" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="373" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="375" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="377" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="379" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="381" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="383" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="385" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="387" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="26" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="168" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="170" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="172" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="174" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="210" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="212" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="214" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="216" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="218" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="220" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="222" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="224" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="244" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="246" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="248" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="250" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="252" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="254" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="256" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="258" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="260" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="262" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="264" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="266" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="268" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="270" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="272" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="274" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="276" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="278" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="280" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="282" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="284" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="286" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="288" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="290" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="292" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="294" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="308" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="310" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="312" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="342" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="344" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="346" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="348" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="350" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="352" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="354" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="356" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="358" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="360" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="362" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="364" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="366" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="368" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="370" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="372" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="374" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="376" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="378" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="380" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="382" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="384" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="386" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -3788,10 +3858,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3810,7 +3880,7 @@
         <v>4096000</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3842,16 +3912,16 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -4390,28 +4460,612 @@
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>17</v>
+      </c>
+      <c r="E22">
+        <v>31</v>
+      </c>
+      <c r="F22">
+        <v>50</v>
+      </c>
+      <c r="G22">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>16.529499999999999</v>
+      </c>
+      <c r="E23">
+        <v>30.1936</v>
+      </c>
+      <c r="F23">
+        <v>45.799399999999999</v>
+      </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>10.1092</v>
+      </c>
+      <c r="E24">
+        <v>19.3932</v>
+      </c>
+      <c r="F24">
+        <v>31.348800000000001</v>
+      </c>
+      <c r="G24">
+        <v>70.274799999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>4.4760200000000001</v>
+      </c>
+      <c r="E25">
+        <v>9.0690200000000001</v>
+      </c>
+      <c r="F25">
+        <v>13.138199999999999</v>
+      </c>
+      <c r="G25">
+        <v>31.618200000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>8</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>2.0501900000000002</v>
+      </c>
+      <c r="E26">
+        <v>4.0399799999999999</v>
+      </c>
+      <c r="F26">
+        <v>6.5367699999999997</v>
+      </c>
+      <c r="G26">
+        <v>15.153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27">
+        <v>10.4048</v>
+      </c>
+      <c r="E27">
+        <v>19.640999999999998</v>
+      </c>
+      <c r="F27">
+        <v>31.046900000000001</v>
+      </c>
+      <c r="G27">
+        <v>69.792699999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>5.4991500000000002</v>
+      </c>
+      <c r="E28">
+        <v>11.831899999999999</v>
+      </c>
+      <c r="F28">
+        <v>16.415199999999999</v>
+      </c>
+      <c r="G28">
+        <v>41.834800000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>2.54644</v>
+      </c>
+      <c r="E29">
+        <v>4.8639999999999999</v>
+      </c>
+      <c r="F29">
+        <v>8.4803099999999993</v>
+      </c>
+      <c r="G29">
+        <v>18.174299999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30">
+        <v>8</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="D30">
+        <v>1.0446599999999999</v>
+      </c>
+      <c r="E30">
+        <v>2.0487700000000002</v>
+      </c>
+      <c r="F30">
+        <v>3.4770099999999999</v>
+      </c>
+      <c r="G30">
+        <v>8.9868000000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>4</v>
+      </c>
+      <c r="D31">
+        <v>6.5306199999999999</v>
+      </c>
+      <c r="E31">
+        <v>15.134600000000001</v>
+      </c>
+      <c r="F31">
+        <v>19.898199999999999</v>
+      </c>
+      <c r="G31">
+        <v>49.162100000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>8</v>
+      </c>
+      <c r="D32">
+        <v>4.0113000000000003</v>
+      </c>
+      <c r="E32">
+        <v>6.3728300000000004</v>
+      </c>
+      <c r="F32">
+        <v>10.598800000000001</v>
+      </c>
+      <c r="G32">
+        <v>28.1051</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>4</v>
+      </c>
+      <c r="C33">
+        <v>16</v>
+      </c>
+      <c r="D33">
+        <v>1.2695799999999999</v>
+      </c>
+      <c r="E33">
+        <v>2.6253099999999998</v>
+      </c>
+      <c r="F33">
+        <v>4.5138800000000003</v>
+      </c>
+      <c r="G33">
+        <v>11.591900000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>8</v>
+      </c>
+      <c r="B34">
+        <v>4</v>
+      </c>
+      <c r="C34">
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <v>0.71308700000000003</v>
+      </c>
+      <c r="E34">
+        <v>1.32935</v>
+      </c>
+      <c r="F34">
+        <v>2.1026699999999998</v>
+      </c>
+      <c r="G34">
+        <v>5.8595800000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>17</v>
+      </c>
+      <c r="E40">
+        <v>31</v>
+      </c>
+      <c r="F40">
+        <v>50</v>
+      </c>
+      <c r="G40">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>5.5999999999999999E-3</v>
+      </c>
+      <c r="E41">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F41">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42">
+        <v>2</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+      <c r="C42">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>6.8635999999999999</v>
+      </c>
+      <c r="E42">
+        <v>10.000400000000001</v>
+      </c>
+      <c r="F42">
+        <v>16.633199999999999</v>
+      </c>
+      <c r="G42">
+        <v>20.400700000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>9.3539499999999993</v>
+      </c>
+      <c r="E43">
+        <v>10.313599999999999</v>
+      </c>
+      <c r="F43">
+        <v>14.864800000000001</v>
+      </c>
+      <c r="G43">
+        <v>16.9848</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>5.94034</v>
+      </c>
+      <c r="E44">
+        <v>8.8614800000000002</v>
+      </c>
+      <c r="F44">
+        <v>21.747399999999999</v>
+      </c>
+      <c r="G44">
+        <v>13.4962</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>26.385000000000002</v>
+      </c>
+      <c r="E45">
+        <v>37.272399999999998</v>
+      </c>
+      <c r="F45">
+        <v>66.886300000000006</v>
+      </c>
+      <c r="G45">
+        <v>114.361</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>19.2149</v>
+      </c>
+      <c r="E46">
+        <v>26.175000000000001</v>
+      </c>
+      <c r="F46">
+        <v>34.636200000000002</v>
+      </c>
+      <c r="G46">
+        <v>46.010399999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47">
+        <v>6.11653</v>
+      </c>
+      <c r="E47">
+        <v>17.061800000000002</v>
+      </c>
+      <c r="F47">
+        <v>25.991499999999998</v>
+      </c>
+      <c r="G47">
+        <v>31.745699999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>16</v>
+      </c>
+      <c r="D48">
+        <v>5.2575099999999999</v>
+      </c>
+      <c r="E48">
+        <v>11.353</v>
+      </c>
+      <c r="F48">
+        <v>11.4354</v>
+      </c>
+      <c r="G48">
+        <v>20.6189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
+      </c>
+      <c r="D49">
+        <v>28.780999999999999</v>
+      </c>
+      <c r="E49">
+        <v>34.027999999999999</v>
+      </c>
+      <c r="F49">
+        <v>49.658700000000003</v>
+      </c>
+      <c r="G49">
+        <v>83.735200000000006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>8</v>
+      </c>
+      <c r="D50">
+        <v>7.9760499999999999</v>
+      </c>
+      <c r="E50">
+        <v>21.449200000000001</v>
+      </c>
+      <c r="F50">
+        <v>26.066099999999999</v>
+      </c>
+      <c r="G50">
+        <v>34.835999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>7.2326899999999998</v>
+      </c>
+      <c r="E51">
+        <v>13.583399999999999</v>
+      </c>
+      <c r="F51">
+        <v>13.250299999999999</v>
+      </c>
+      <c r="G51">
+        <v>27.873799999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52">
+        <v>8</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>32</v>
+      </c>
+      <c r="D52">
+        <v>5.7665499999999996</v>
+      </c>
+      <c r="E52">
+        <v>5.6740300000000001</v>
+      </c>
+      <c r="F52">
+        <v>10.313599999999999</v>
+      </c>
+      <c r="G52">
+        <v>12.511100000000001</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A3:G14">
@@ -4429,10 +5083,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB22"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3:U14"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4448,14 +5102,17 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="R1" t="s">
         <v>1</v>
       </c>
       <c r="Y1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:28">
@@ -4487,16 +5144,16 @@
         <v>3</v>
       </c>
       <c r="K2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="P2" t="s">
         <v>4</v>
@@ -4505,16 +5162,16 @@
         <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="S2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="T2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="U2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="W2" t="s">
         <v>4</v>
@@ -4523,16 +5180,16 @@
         <v>3</v>
       </c>
       <c r="Y2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="Z2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AA2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AB2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:28">
@@ -5607,18 +6264,888 @@
         <v>0.10926780736690819</v>
       </c>
     </row>
-    <row r="21" spans="11:14">
-      <c r="K21">
-        <f>57/208</f>
-        <v>0.27403846153846156</v>
-      </c>
-      <c r="N21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="11:14">
-      <c r="N22" t="s">
-        <v>20</v>
+    <row r="19" spans="1:23">
+      <c r="B19">
+        <v>4096000</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+      <c r="R19" t="s">
+        <v>25</v>
+      </c>
+      <c r="W19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
+        <v>31</v>
+      </c>
+      <c r="F20">
+        <v>50</v>
+      </c>
+      <c r="G20">
+        <v>101</v>
+      </c>
+      <c r="I20" t="s">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>3</v>
+      </c>
+      <c r="K20" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" t="s">
+        <v>9</v>
+      </c>
+      <c r="M20" t="s">
+        <v>10</v>
+      </c>
+      <c r="N20" t="s">
+        <v>11</v>
+      </c>
+      <c r="P20" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" t="s">
+        <v>9</v>
+      </c>
+      <c r="T20" t="s">
+        <v>10</v>
+      </c>
+      <c r="U20" t="s">
+        <v>11</v>
+      </c>
+      <c r="W20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21" s="8">
+        <f>D21/D3</f>
+        <v>2.0571233236276179E-3</v>
+      </c>
+      <c r="L21" s="8">
+        <f t="shared" ref="L21:N21" si="4">E21/E3</f>
+        <v>1.1419895702686647E-3</v>
+      </c>
+      <c r="M21" s="8">
+        <f t="shared" si="4"/>
+        <v>7.4612698286556894E-4</v>
+      </c>
+      <c r="N21" s="8" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P21">
+        <v>1</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21" s="8">
+        <f>(m2070_nooverlap_vcl!D3-D3)/m2070_nooverlap_vcl!D3</f>
+        <v>9.4147951964589915E-3</v>
+      </c>
+      <c r="S21" s="8">
+        <f>(m2070_nooverlap_vcl!E3-E3)/m2070_nooverlap_vcl!E3</f>
+        <v>-3.1819190183399008E-3</v>
+      </c>
+      <c r="T21" s="8">
+        <f>(m2070_nooverlap_vcl!F3-F3)/m2070_nooverlap_vcl!F3</f>
+        <v>1.1074508982075007E-2</v>
+      </c>
+      <c r="U21" s="8" t="e">
+        <f>(m2070_nooverlap_vcl!G3-G3)/m2070_nooverlap_vcl!G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" s="6">
+        <v>6.54765</v>
+      </c>
+      <c r="E22" s="6">
+        <v>8.9044000000000008</v>
+      </c>
+      <c r="F22" s="6">
+        <v>16.738700000000001</v>
+      </c>
+      <c r="G22" s="6">
+        <v>19.728300000000001</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="8">
+        <f t="shared" ref="K22:N22" si="5">D22/D4</f>
+        <v>0.64773064519320189</v>
+      </c>
+      <c r="L22" s="8">
+        <f t="shared" si="5"/>
+        <v>0.45691004346197467</v>
+      </c>
+      <c r="M22" s="8">
+        <f t="shared" si="5"/>
+        <v>0.53526842246639128</v>
+      </c>
+      <c r="N22" s="8">
+        <f t="shared" si="5"/>
+        <v>0.32088502282822795</v>
+      </c>
+      <c r="P22">
+        <v>2</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22" s="8">
+        <f>(m2070_nooverlap_vcl!D4-D4)/m2070_nooverlap_vcl!D4</f>
+        <v>0.55860533152850256</v>
+      </c>
+      <c r="S22" s="8">
+        <f>(m2070_nooverlap_vcl!E4-E4)/m2070_nooverlap_vcl!E4</f>
+        <v>0.47846786236130967</v>
+      </c>
+      <c r="T22" s="8">
+        <f>(m2070_nooverlap_vcl!F4-F4)/m2070_nooverlap_vcl!F4</f>
+        <v>0.51110089692057792</v>
+      </c>
+      <c r="U22" s="8">
+        <f>(m2070_nooverlap_vcl!G4-G4)/m2070_nooverlap_vcl!G4</f>
+        <v>0.43586188544897325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6">
+        <v>9.6577500000000001</v>
+      </c>
+      <c r="E23" s="6">
+        <v>8.8386999999999993</v>
+      </c>
+      <c r="F23" s="6">
+        <v>15.0204</v>
+      </c>
+      <c r="G23" s="6">
+        <v>14.6511</v>
+      </c>
+      <c r="I23">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" s="8">
+        <f t="shared" ref="K23:N23" si="6">D23/D5</f>
+        <v>0.91059306053177447</v>
+      </c>
+      <c r="L23" s="8">
+        <f t="shared" si="6"/>
+        <v>0.87459924797150201</v>
+      </c>
+      <c r="M23" s="8">
+        <f t="shared" si="6"/>
+        <v>0.90222366381951213</v>
+      </c>
+      <c r="N23" s="8">
+        <f t="shared" si="6"/>
+        <v>0.44682564129151892</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="8">
+        <f>(m2070_nooverlap_vcl!D5-D5)/m2070_nooverlap_vcl!D5</f>
+        <v>0.47184694218003814</v>
+      </c>
+      <c r="S23" s="8">
+        <f>(m2070_nooverlap_vcl!E5-E5)/m2070_nooverlap_vcl!E5</f>
+        <v>0.63673746679559029</v>
+      </c>
+      <c r="T23" s="8">
+        <f>(m2070_nooverlap_vcl!F5-F5)/m2070_nooverlap_vcl!F5</f>
+        <v>0.58184640424377598</v>
+      </c>
+      <c r="U23" s="8">
+        <f>(m2070_nooverlap_vcl!G5-G5)/m2070_nooverlap_vcl!G5</f>
+        <v>0.47203785822166838</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24" s="6">
+        <v>4.8533499999999998</v>
+      </c>
+      <c r="E24" s="6">
+        <v>6.5807599999999997</v>
+      </c>
+      <c r="F24" s="6">
+        <v>8.6257599999999996</v>
+      </c>
+      <c r="G24" s="6">
+        <v>10.151300000000001</v>
+      </c>
+      <c r="I24">
+        <v>8</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" s="8">
+        <f t="shared" ref="K24:N24" si="7">D24/D6</f>
+        <v>0.85357188709674581</v>
+      </c>
+      <c r="L24" s="8">
+        <f t="shared" si="7"/>
+        <v>0.85933702883931085</v>
+      </c>
+      <c r="M24" s="8">
+        <f t="shared" si="7"/>
+        <v>0.86787961231083144</v>
+      </c>
+      <c r="N24" s="8">
+        <f t="shared" si="7"/>
+        <v>0.6570718414426544</v>
+      </c>
+      <c r="P24">
+        <v>8</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24" s="8">
+        <f>(m2070_nooverlap_vcl!D6-D6)/m2070_nooverlap_vcl!D6</f>
+        <v>0.50435157823164833</v>
+      </c>
+      <c r="S24" s="8">
+        <f>(m2070_nooverlap_vcl!E6-E6)/m2070_nooverlap_vcl!E6</f>
+        <v>0.55891196037208768</v>
+      </c>
+      <c r="T24" s="8">
+        <f>(m2070_nooverlap_vcl!F6-F6)/m2070_nooverlap_vcl!F6</f>
+        <v>0.70567919002395696</v>
+      </c>
+      <c r="U24" s="8">
+        <f>(m2070_nooverlap_vcl!G6-G6)/m2070_nooverlap_vcl!G6</f>
+        <v>0.57090879801803651</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>9.1751500000000004</v>
+      </c>
+      <c r="E25" s="6">
+        <v>13.3239</v>
+      </c>
+      <c r="F25" s="6">
+        <v>23.316299999999998</v>
+      </c>
+      <c r="G25" s="6">
+        <v>38.147199999999998</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25" s="8">
+        <f t="shared" ref="K25:N25" si="8">D25/D7</f>
+        <v>0.74543201852378438</v>
+      </c>
+      <c r="L25" s="8">
+        <f t="shared" si="8"/>
+        <v>0.63914019552349066</v>
+      </c>
+      <c r="M25" s="8">
+        <f t="shared" si="8"/>
+        <v>0.68879002454868521</v>
+      </c>
+      <c r="N25" s="8">
+        <f t="shared" si="8"/>
+        <v>0.58495953285674418</v>
+      </c>
+      <c r="P25">
+        <v>1</v>
+      </c>
+      <c r="Q25">
+        <v>2</v>
+      </c>
+      <c r="R25" s="8">
+        <f>(m2070_nooverlap_vcl!D7-D7)/m2070_nooverlap_vcl!D7</f>
+        <v>0.70160488739120941</v>
+      </c>
+      <c r="S25" s="8">
+        <f>(m2070_nooverlap_vcl!E7-E7)/m2070_nooverlap_vcl!E7</f>
+        <v>0.66534441435352776</v>
+      </c>
+      <c r="T25" s="8">
+        <f>(m2070_nooverlap_vcl!F7-F7)/m2070_nooverlap_vcl!F7</f>
+        <v>0.6905155468600005</v>
+      </c>
+      <c r="U25" s="8">
+        <f>(m2070_nooverlap_vcl!G7-G7)/m2070_nooverlap_vcl!G7</f>
+        <v>0.67023634947764432</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6">
+        <v>9.5302699999999998</v>
+      </c>
+      <c r="E26" s="6">
+        <v>9.6920999999999999</v>
+      </c>
+      <c r="F26" s="6">
+        <v>15.897600000000001</v>
+      </c>
+      <c r="G26" s="6">
+        <v>19.348500000000001</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26" s="8">
+        <f t="shared" ref="K26:N26" si="9">D26/D8</f>
+        <v>0.89007219373698321</v>
+      </c>
+      <c r="L26" s="8">
+        <f t="shared" si="9"/>
+        <v>0.87294196058651874</v>
+      </c>
+      <c r="M26" s="8">
+        <f t="shared" si="9"/>
+        <v>0.89697858775072636</v>
+      </c>
+      <c r="N26" s="8">
+        <f t="shared" si="9"/>
+        <v>0.57387211299187035</v>
+      </c>
+      <c r="P26">
+        <v>2</v>
+      </c>
+      <c r="Q26">
+        <v>2</v>
+      </c>
+      <c r="R26" s="8">
+        <f>(m2070_nooverlap_vcl!D8-D8)/m2070_nooverlap_vcl!D8</f>
+        <v>0.66414371122249893</v>
+      </c>
+      <c r="S26" s="8">
+        <f>(m2070_nooverlap_vcl!E8-E8)/m2070_nooverlap_vcl!E8</f>
+        <v>0.76261764567538559</v>
+      </c>
+      <c r="T26" s="8">
+        <f>(m2070_nooverlap_vcl!F8-F8)/m2070_nooverlap_vcl!F8</f>
+        <v>0.71869826824092575</v>
+      </c>
+      <c r="U26" s="8">
+        <f>(m2070_nooverlap_vcl!G8-G8)/m2070_nooverlap_vcl!G8</f>
+        <v>0.66862222833778895</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6">
+        <v>4.5308400000000004</v>
+      </c>
+      <c r="E27" s="6">
+        <v>5.5327099999999998</v>
+      </c>
+      <c r="F27" s="6">
+        <v>6.7210400000000003</v>
+      </c>
+      <c r="G27" s="6">
+        <v>10.5749</v>
+      </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27" s="8">
+        <f t="shared" ref="K27:N27" si="10">D27/D9</f>
+        <v>0.81750175919744517</v>
+      </c>
+      <c r="L27" s="8">
+        <f t="shared" si="10"/>
+        <v>0.82281180520958042</v>
+      </c>
+      <c r="M27" s="8">
+        <f t="shared" si="10"/>
+        <v>0.82167919370534659</v>
+      </c>
+      <c r="N27" s="8">
+        <f t="shared" si="10"/>
+        <v>0.68406106475192441</v>
+      </c>
+      <c r="P27">
+        <v>4</v>
+      </c>
+      <c r="Q27">
+        <v>2</v>
+      </c>
+      <c r="R27" s="8">
+        <f>(m2070_nooverlap_vcl!D9-D9)/m2070_nooverlap_vcl!D9</f>
+        <v>0.55765286169219352</v>
+      </c>
+      <c r="S27" s="8">
+        <f>(m2070_nooverlap_vcl!E9-E9)/m2070_nooverlap_vcl!E9</f>
+        <v>0.75464142103381082</v>
+      </c>
+      <c r="T27" s="8">
+        <f>(m2070_nooverlap_vcl!F9-F9)/m2070_nooverlap_vcl!F9</f>
+        <v>0.80167781166806484</v>
+      </c>
+      <c r="U27" s="8">
+        <f>(m2070_nooverlap_vcl!G9-G9)/m2070_nooverlap_vcl!G9</f>
+        <v>0.73524394755230382</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28">
+        <v>8</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>16</v>
+      </c>
+      <c r="D28" s="6">
+        <v>3.5802</v>
+      </c>
+      <c r="E28" s="6">
+        <v>5.5792200000000003</v>
+      </c>
+      <c r="F28" s="6">
+        <v>5.5587600000000004</v>
+      </c>
+      <c r="G28" s="6">
+        <v>7.2564399999999996</v>
+      </c>
+      <c r="I28">
+        <v>8</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28" s="8">
+        <f t="shared" ref="K28:N28" si="11">D28/D10</f>
+        <v>0.9209991510817277</v>
+      </c>
+      <c r="L28" s="8">
+        <f t="shared" si="11"/>
+        <v>0.84166491923865439</v>
+      </c>
+      <c r="M28" s="8">
+        <f t="shared" si="11"/>
+        <v>0.80885986432568824</v>
+      </c>
+      <c r="N28" s="8">
+        <f t="shared" si="11"/>
+        <v>0.76816337937517465</v>
+      </c>
+      <c r="P28">
+        <v>8</v>
+      </c>
+      <c r="Q28">
+        <v>2</v>
+      </c>
+      <c r="R28" s="8">
+        <f>(m2070_nooverlap_vcl!D10-D10)/m2070_nooverlap_vcl!D10</f>
+        <v>0.55489780729375393</v>
+      </c>
+      <c r="S28" s="8">
+        <f>(m2070_nooverlap_vcl!E10-E10)/m2070_nooverlap_vcl!E10</f>
+        <v>0.59782372605764966</v>
+      </c>
+      <c r="T28" s="8">
+        <f>(m2070_nooverlap_vcl!F10-F10)/m2070_nooverlap_vcl!F10</f>
+        <v>0.62699586958527587</v>
+      </c>
+      <c r="U28" s="8">
+        <f>(m2070_nooverlap_vcl!G10-G10)/m2070_nooverlap_vcl!G10</f>
+        <v>0.72765805322593202</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="6">
+        <v>8.4573199999999993</v>
+      </c>
+      <c r="E29" s="6">
+        <v>9.4307800000000004</v>
+      </c>
+      <c r="F29" s="6">
+        <v>11.8721</v>
+      </c>
+      <c r="G29" s="6">
+        <v>17.736000000000001</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29" s="8">
+        <f t="shared" ref="K29:N29" si="12">D29/D11</f>
+        <v>0.85400733103775572</v>
+      </c>
+      <c r="L29" s="8">
+        <f t="shared" si="12"/>
+        <v>0.83661831891772009</v>
+      </c>
+      <c r="M29" s="8">
+        <f t="shared" si="12"/>
+        <v>0.80856642761307373</v>
+      </c>
+      <c r="N29" s="8">
+        <f t="shared" si="12"/>
+        <v>0.52321979597496004</v>
+      </c>
+      <c r="P29">
+        <v>1</v>
+      </c>
+      <c r="Q29">
+        <v>4</v>
+      </c>
+      <c r="R29" s="8">
+        <f>(m2070_nooverlap_vcl!D11-D11)/m2070_nooverlap_vcl!D11</f>
+        <v>0.76780702597637063</v>
+      </c>
+      <c r="S29" s="8">
+        <f>(m2070_nooverlap_vcl!E11-E11)/m2070_nooverlap_vcl!E11</f>
+        <v>0.80262777761241333</v>
+      </c>
+      <c r="T29" s="8">
+        <f>(m2070_nooverlap_vcl!F11-F11)/m2070_nooverlap_vcl!F11</f>
+        <v>0.81555350655484815</v>
+      </c>
+      <c r="U29" s="8">
+        <f>(m2070_nooverlap_vcl!G11-G11)/m2070_nooverlap_vcl!G11</f>
+        <v>0.77291405679526781</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30" s="6">
+        <v>5.0602600000000004</v>
+      </c>
+      <c r="E30" s="6">
+        <v>6.3272500000000003</v>
+      </c>
+      <c r="F30" s="6">
+        <v>8.9269599999999993</v>
+      </c>
+      <c r="G30" s="6">
+        <v>9.9823199999999996</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30" s="8">
+        <f t="shared" ref="K30:N30" si="13">D30/D12</f>
+        <v>0.7126434191606732</v>
+      </c>
+      <c r="L30" s="8">
+        <f t="shared" si="13"/>
+        <v>0.79707461114701406</v>
+      </c>
+      <c r="M30" s="8">
+        <f t="shared" si="13"/>
+        <v>0.81101097463478455</v>
+      </c>
+      <c r="N30" s="8">
+        <f t="shared" si="13"/>
+        <v>0.6125851467285246</v>
+      </c>
+      <c r="P30">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>4</v>
+      </c>
+      <c r="R30" s="8">
+        <f>(m2070_nooverlap_vcl!D12-D12)/m2070_nooverlap_vcl!D12</f>
+        <v>0.5768714171642414</v>
+      </c>
+      <c r="S30" s="8">
+        <f>(m2070_nooverlap_vcl!E12-E12)/m2070_nooverlap_vcl!E12</f>
+        <v>0.76189349218918723</v>
+      </c>
+      <c r="T30" s="8">
+        <f>(m2070_nooverlap_vcl!F12-F12)/m2070_nooverlap_vcl!F12</f>
+        <v>0.74510398743953077</v>
+      </c>
+      <c r="U30" s="8">
+        <f>(m2070_nooverlap_vcl!G12-G12)/m2070_nooverlap_vcl!G12</f>
+        <v>0.78374009634908626</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+      <c r="D31" s="6">
+        <v>4.2336799999999997</v>
+      </c>
+      <c r="E31" s="6">
+        <v>5.2179700000000002</v>
+      </c>
+      <c r="F31" s="6">
+        <v>5.44611</v>
+      </c>
+      <c r="G31" s="6">
+        <v>7.6630099999999999</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31" s="8">
+        <f t="shared" ref="K31:N31" si="14">D31/D13</f>
+        <v>0.83665266211617573</v>
+      </c>
+      <c r="L31" s="8">
+        <f t="shared" si="14"/>
+        <v>0.79287562660783129</v>
+      </c>
+      <c r="M31" s="8">
+        <f t="shared" si="14"/>
+        <v>0.75790840431912776</v>
+      </c>
+      <c r="N31" s="8">
+        <f t="shared" si="14"/>
+        <v>0.75297337132750319</v>
+      </c>
+      <c r="P31">
+        <v>4</v>
+      </c>
+      <c r="Q31">
+        <v>4</v>
+      </c>
+      <c r="R31" s="8">
+        <f>(m2070_nooverlap_vcl!D13-D13)/m2070_nooverlap_vcl!D13</f>
+        <v>0.55049079264121947</v>
+      </c>
+      <c r="S31" s="8">
+        <f>(m2070_nooverlap_vcl!E13-E13)/m2070_nooverlap_vcl!E13</f>
+        <v>0.6667559561485682</v>
+      </c>
+      <c r="T31" s="8">
+        <f>(m2070_nooverlap_vcl!F13-F13)/m2070_nooverlap_vcl!F13</f>
+        <v>0.67143079237483827</v>
+      </c>
+      <c r="U31" s="8">
+        <f>(m2070_nooverlap_vcl!G13-G13)/m2070_nooverlap_vcl!G13</f>
+        <v>0.77877914433155526</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>32</v>
+      </c>
+      <c r="D32" s="6">
+        <v>2.35283</v>
+      </c>
+      <c r="E32" s="6">
+        <v>2.8033199999999998</v>
+      </c>
+      <c r="F32" s="6">
+        <v>3.1852900000000002</v>
+      </c>
+      <c r="G32" s="6">
+        <v>4.07925</v>
+      </c>
+      <c r="I32">
+        <v>8</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32" s="8">
+        <f t="shared" ref="K32:N32" si="15">D32/D14</f>
+        <v>0.85963200853482991</v>
+      </c>
+      <c r="L32" s="8">
+        <f t="shared" si="15"/>
+        <v>0.6803943555316081</v>
+      </c>
+      <c r="M32" s="8">
+        <f t="shared" si="15"/>
+        <v>0.69053436206720875</v>
+      </c>
+      <c r="N32" s="8">
+        <f t="shared" si="15"/>
+        <v>0.64496416470480356</v>
+      </c>
+      <c r="P32">
+        <v>8</v>
+      </c>
+      <c r="Q32">
+        <v>4</v>
+      </c>
+      <c r="R32" s="8">
+        <f>(m2070_nooverlap_vcl!D14-D14)/m2070_nooverlap_vcl!D14</f>
+        <v>0.65770092258744695</v>
+      </c>
+      <c r="S32" s="8">
+        <f>(m2070_nooverlap_vcl!E14-E14)/m2070_nooverlap_vcl!E14</f>
+        <v>0.53847549746618206</v>
+      </c>
+      <c r="T32" s="8">
+        <f>(m2070_nooverlap_vcl!F14-F14)/m2070_nooverlap_vcl!F14</f>
+        <v>0.68427821468416117</v>
+      </c>
+      <c r="U32" s="8">
+        <f>(m2070_nooverlap_vcl!G14-G14)/m2070_nooverlap_vcl!G14</f>
+        <v>0.71400542618132479</v>
       </c>
     </row>
   </sheetData>
@@ -5664,25 +7191,25 @@
   <sheetData>
     <row r="1" spans="1:25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B1" s="4">
         <v>17</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H1" s="4">
         <v>31</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="O1" s="4">
         <v>50</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V1" s="4">
         <v>101</v>
@@ -5690,33 +7217,33 @@
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="U3" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -5728,10 +7255,10 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -5743,10 +7270,10 @@
         <v>4</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="O4">
         <v>1</v>
@@ -5758,10 +7285,10 @@
         <v>4</v>
       </c>
       <c r="R4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="U4" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="V4">
         <v>1</v>
@@ -5773,7 +7300,7 @@
         <v>4</v>
       </c>
       <c r="Y4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:25">
@@ -6026,7 +7553,7 @@
     </row>
     <row r="9" spans="1:25">
       <c r="A9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B9" s="5" t="e">
         <v>#DIV/0!</v>
@@ -6041,7 +7568,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H9" s="5">
         <v>38.960233472592222</v>
@@ -6056,7 +7583,7 @@
         <v>126.51070204580169</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="O9" s="5">
         <v>37.728343536244417</v>
@@ -6071,7 +7598,7 @@
         <v>141.53147432681851</v>
       </c>
       <c r="U9" s="4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="V9" s="5" t="e">
         <v>#DIV/0!</v>
@@ -6113,22 +7640,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
adding new data and references
</commit_message>
<xml_diff>
--- a/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
+++ b/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26540" windowHeight="14920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="m2070_nooverlap_vcl" sheetId="1" r:id="rId1"/>
@@ -161,9 +161,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="394">
+  <cellStyleXfs count="400">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -570,7 +576,7 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="394">
+  <cellStyles count="400">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -767,6 +773,9 @@
     <cellStyle name="Followed Hyperlink" xfId="389" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="391" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="393" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="395" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="397" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="399" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -963,6 +972,9 @@
     <cellStyle name="Hyperlink" xfId="388" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="390" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="392" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="394" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="396" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="398" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -3861,7 +3873,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5085,8 +5097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21:U32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6395,19 +6407,19 @@
         <v>1</v>
       </c>
       <c r="R21" s="8">
-        <f>(m2070_nooverlap_vcl!D3-D3)/m2070_nooverlap_vcl!D3</f>
-        <v>9.4147951964589915E-3</v>
+        <f>D3/m2070_nooverlap_vcl!D23</f>
+        <v>0.99108260987930685</v>
       </c>
       <c r="S21" s="8">
-        <f>(m2070_nooverlap_vcl!E3-E3)/m2070_nooverlap_vcl!E3</f>
-        <v>-3.1819190183399008E-3</v>
+        <f>E3/m2070_nooverlap_vcl!E23</f>
+        <v>1.0034576863971172</v>
       </c>
       <c r="T21" s="8">
-        <f>(m2070_nooverlap_vcl!F3-F3)/m2070_nooverlap_vcl!F3</f>
-        <v>1.1074508982075007E-2</v>
+        <f>F3/m2070_nooverlap_vcl!F23</f>
+        <v>0.98910902762918296</v>
       </c>
       <c r="U21" s="8" t="e">
-        <f>(m2070_nooverlap_vcl!G3-G3)/m2070_nooverlap_vcl!G3</f>
+        <f>G3/m2070_nooverlap_vcl!G23</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6462,20 +6474,20 @@
         <v>1</v>
       </c>
       <c r="R22" s="8">
-        <f>(m2070_nooverlap_vcl!D4-D4)/m2070_nooverlap_vcl!D4</f>
-        <v>0.55860533152850256</v>
+        <f>D4/m2070_nooverlap_vcl!D24</f>
+        <v>0.99994064812250227</v>
       </c>
       <c r="S22" s="8">
-        <f>(m2070_nooverlap_vcl!E4-E4)/m2070_nooverlap_vcl!E4</f>
-        <v>0.47846786236130967</v>
+        <f>E4/m2070_nooverlap_vcl!E24</f>
+        <v>1.0049037807066394</v>
       </c>
       <c r="T22" s="8">
-        <f>(m2070_nooverlap_vcl!F4-F4)/m2070_nooverlap_vcl!F4</f>
-        <v>0.51110089692057792</v>
+        <f>F4/m2070_nooverlap_vcl!F24</f>
+        <v>0.99753738580105134</v>
       </c>
       <c r="U22" s="8">
-        <f>(m2070_nooverlap_vcl!G4-G4)/m2070_nooverlap_vcl!G4</f>
-        <v>0.43586188544897325</v>
+        <f>G4/m2070_nooverlap_vcl!G24</f>
+        <v>0.87486410491385247</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -6529,20 +6541,20 @@
         <v>1</v>
       </c>
       <c r="R23" s="8">
-        <f>(m2070_nooverlap_vcl!D5-D5)/m2070_nooverlap_vcl!D5</f>
-        <v>0.47184694218003814</v>
+        <f>D5/m2070_nooverlap_vcl!D25</f>
+        <v>2.3695157751752673</v>
       </c>
       <c r="S23" s="8">
-        <f>(m2070_nooverlap_vcl!E5-E5)/m2070_nooverlap_vcl!E5</f>
-        <v>0.63673746679559029</v>
+        <f>E5/m2070_nooverlap_vcl!E25</f>
+        <v>1.1143431153531473</v>
       </c>
       <c r="T23" s="8">
-        <f>(m2070_nooverlap_vcl!F5-F5)/m2070_nooverlap_vcl!F5</f>
-        <v>0.58184640424377598</v>
+        <f>F5/m2070_nooverlap_vcl!F25</f>
+        <v>1.2671598849157419</v>
       </c>
       <c r="U23" s="8">
-        <f>(m2070_nooverlap_vcl!G5-G5)/m2070_nooverlap_vcl!G5</f>
-        <v>0.47203785822166838</v>
+        <f>G5/m2070_nooverlap_vcl!G25</f>
+        <v>1.0370387941122516</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -6596,20 +6608,20 @@
         <v>1</v>
       </c>
       <c r="R24" s="8">
-        <f>(m2070_nooverlap_vcl!D6-D6)/m2070_nooverlap_vcl!D6</f>
-        <v>0.50435157823164833</v>
+        <f>D6/m2070_nooverlap_vcl!D26</f>
+        <v>2.7733673464410611</v>
       </c>
       <c r="S24" s="8">
-        <f>(m2070_nooverlap_vcl!E6-E6)/m2070_nooverlap_vcl!E6</f>
-        <v>0.55891196037208768</v>
+        <f>E6/m2070_nooverlap_vcl!E26</f>
+        <v>1.8955415620869409</v>
       </c>
       <c r="T24" s="8">
-        <f>(m2070_nooverlap_vcl!F6-F6)/m2070_nooverlap_vcl!F6</f>
-        <v>0.70567919002395696</v>
+        <f>F6/m2070_nooverlap_vcl!F26</f>
+        <v>1.520458881068173</v>
       </c>
       <c r="U24" s="8">
-        <f>(m2070_nooverlap_vcl!G6-G6)/m2070_nooverlap_vcl!G6</f>
-        <v>0.57090879801803651</v>
+        <f>G6/m2070_nooverlap_vcl!G26</f>
+        <v>1.0195538837193954</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -6663,20 +6675,20 @@
         <v>2</v>
       </c>
       <c r="R25" s="8">
-        <f>(m2070_nooverlap_vcl!D7-D7)/m2070_nooverlap_vcl!D7</f>
-        <v>0.70160488739120941</v>
+        <f>D7/m2070_nooverlap_vcl!D27</f>
+        <v>1.1829636321697679</v>
       </c>
       <c r="S25" s="8">
-        <f>(m2070_nooverlap_vcl!E7-E7)/m2070_nooverlap_vcl!E7</f>
-        <v>0.66534441435352776</v>
+        <f>E7/m2070_nooverlap_vcl!E27</f>
+        <v>1.0613818033705005</v>
       </c>
       <c r="T25" s="8">
-        <f>(m2070_nooverlap_vcl!F7-F7)/m2070_nooverlap_vcl!F7</f>
-        <v>0.6905155468600005</v>
+        <f>F7/m2070_nooverlap_vcl!F27</f>
+        <v>1.0903214169530613</v>
       </c>
       <c r="U25" s="8">
-        <f>(m2070_nooverlap_vcl!G7-G7)/m2070_nooverlap_vcl!G7</f>
-        <v>0.67023634947764432</v>
+        <f>G7/m2070_nooverlap_vcl!G27</f>
+        <v>0.93438712071606334</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -6730,20 +6742,20 @@
         <v>2</v>
       </c>
       <c r="R26" s="8">
-        <f>(m2070_nooverlap_vcl!D8-D8)/m2070_nooverlap_vcl!D8</f>
-        <v>0.66414371122249893</v>
+        <f>D8/m2070_nooverlap_vcl!D28</f>
+        <v>1.9470827309675132</v>
       </c>
       <c r="S26" s="8">
-        <f>(m2070_nooverlap_vcl!E8-E8)/m2070_nooverlap_vcl!E8</f>
-        <v>0.76261764567538559</v>
+        <f>E8/m2070_nooverlap_vcl!E28</f>
+        <v>0.93837845147440402</v>
       </c>
       <c r="T26" s="8">
-        <f>(m2070_nooverlap_vcl!F8-F8)/m2070_nooverlap_vcl!F8</f>
-        <v>0.71869826824092575</v>
+        <f>F8/m2070_nooverlap_vcl!F28</f>
+        <v>1.0797005214679081</v>
       </c>
       <c r="U26" s="8">
-        <f>(m2070_nooverlap_vcl!G8-G8)/m2070_nooverlap_vcl!G8</f>
-        <v>0.66862222833778895</v>
+        <f>G8/m2070_nooverlap_vcl!G28</f>
+        <v>0.80592473251933794</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -6797,20 +6809,20 @@
         <v>2</v>
       </c>
       <c r="R27" s="8">
-        <f>(m2070_nooverlap_vcl!D9-D9)/m2070_nooverlap_vcl!D9</f>
-        <v>0.55765286169219352</v>
+        <f>D9/m2070_nooverlap_vcl!D29</f>
+        <v>2.1764895304817706</v>
       </c>
       <c r="S27" s="8">
-        <f>(m2070_nooverlap_vcl!E9-E9)/m2070_nooverlap_vcl!E9</f>
-        <v>0.75464142103381082</v>
+        <f>E9/m2070_nooverlap_vcl!E29</f>
+        <v>1.3824321546052631</v>
       </c>
       <c r="T27" s="8">
-        <f>(m2070_nooverlap_vcl!F9-F9)/m2070_nooverlap_vcl!F9</f>
-        <v>0.80167781166806484</v>
+        <f>F9/m2070_nooverlap_vcl!F29</f>
+        <v>0.9645449281924835</v>
       </c>
       <c r="U27" s="8">
-        <f>(m2070_nooverlap_vcl!G9-G9)/m2070_nooverlap_vcl!G9</f>
-        <v>0.73524394755230382</v>
+        <f>G9/m2070_nooverlap_vcl!G29</f>
+        <v>0.85059672174444134</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -6864,20 +6876,20 @@
         <v>2</v>
       </c>
       <c r="R28" s="8">
-        <f>(m2070_nooverlap_vcl!D10-D10)/m2070_nooverlap_vcl!D10</f>
-        <v>0.55489780729375393</v>
+        <f>D10/m2070_nooverlap_vcl!D30</f>
+        <v>3.7211150039247225</v>
       </c>
       <c r="S28" s="8">
-        <f>(m2070_nooverlap_vcl!E10-E10)/m2070_nooverlap_vcl!E10</f>
-        <v>0.59782372605764966</v>
+        <f>E10/m2070_nooverlap_vcl!E30</f>
+        <v>3.2354973959985744</v>
       </c>
       <c r="T28" s="8">
-        <f>(m2070_nooverlap_vcl!F10-F10)/m2070_nooverlap_vcl!F10</f>
-        <v>0.62699586958527587</v>
+        <f>F10/m2070_nooverlap_vcl!F30</f>
+        <v>1.9765085518879728</v>
       </c>
       <c r="U28" s="8">
-        <f>(m2070_nooverlap_vcl!G10-G10)/m2070_nooverlap_vcl!G10</f>
-        <v>0.72765805322593202</v>
+        <f>G10/m2070_nooverlap_vcl!G30</f>
+        <v>1.0511505764009434</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -6931,20 +6943,20 @@
         <v>4</v>
       </c>
       <c r="R29" s="8">
-        <f>(m2070_nooverlap_vcl!D11-D11)/m2070_nooverlap_vcl!D11</f>
-        <v>0.76780702597637063</v>
+        <f>D11/m2070_nooverlap_vcl!D31</f>
+        <v>1.5164103867626657</v>
       </c>
       <c r="S29" s="8">
-        <f>(m2070_nooverlap_vcl!E11-E11)/m2070_nooverlap_vcl!E11</f>
-        <v>0.80262777761241333</v>
+        <f>E11/m2070_nooverlap_vcl!E31</f>
+        <v>0.74481651315528663</v>
       </c>
       <c r="T29" s="8">
-        <f>(m2070_nooverlap_vcl!F11-F11)/m2070_nooverlap_vcl!F11</f>
-        <v>0.81555350655484815</v>
+        <f>F11/m2070_nooverlap_vcl!F31</f>
+        <v>0.73790091566071303</v>
       </c>
       <c r="U29" s="8">
-        <f>(m2070_nooverlap_vcl!G11-G11)/m2070_nooverlap_vcl!G11</f>
-        <v>0.77291405679526781</v>
+        <f>G11/m2070_nooverlap_vcl!G31</f>
+        <v>0.68951082236112771</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -6998,20 +7010,20 @@
         <v>4</v>
       </c>
       <c r="R30" s="8">
-        <f>(m2070_nooverlap_vcl!D12-D12)/m2070_nooverlap_vcl!D12</f>
-        <v>0.5768714171642414</v>
+        <f>D12/m2070_nooverlap_vcl!D32</f>
+        <v>1.7701717647645401</v>
       </c>
       <c r="S30" s="8">
-        <f>(m2070_nooverlap_vcl!E12-E12)/m2070_nooverlap_vcl!E12</f>
-        <v>0.76189349218918723</v>
+        <f>E12/m2070_nooverlap_vcl!E32</f>
+        <v>1.2456145856707301</v>
       </c>
       <c r="T30" s="8">
-        <f>(m2070_nooverlap_vcl!F12-F12)/m2070_nooverlap_vcl!F12</f>
-        <v>0.74510398743953077</v>
+        <f>F12/m2070_nooverlap_vcl!F32</f>
+        <v>1.0385326640751782</v>
       </c>
       <c r="U30" s="8">
-        <f>(m2070_nooverlap_vcl!G12-G12)/m2070_nooverlap_vcl!G12</f>
-        <v>0.78374009634908626</v>
+        <f>G12/m2070_nooverlap_vcl!G32</f>
+        <v>0.57980224229766131</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -7065,20 +7077,20 @@
         <v>4</v>
       </c>
       <c r="R31" s="8">
-        <f>(m2070_nooverlap_vcl!D13-D13)/m2070_nooverlap_vcl!D13</f>
-        <v>0.55049079264121947</v>
+        <f>D13/m2070_nooverlap_vcl!D33</f>
+        <v>3.9857748231698675</v>
       </c>
       <c r="S31" s="8">
-        <f>(m2070_nooverlap_vcl!E13-E13)/m2070_nooverlap_vcl!E13</f>
-        <v>0.6667559561485682</v>
+        <f>E13/m2070_nooverlap_vcl!E33</f>
+        <v>2.5067782471403381</v>
       </c>
       <c r="T31" s="8">
-        <f>(m2070_nooverlap_vcl!F13-F13)/m2070_nooverlap_vcl!F13</f>
-        <v>0.67143079237483827</v>
+        <f>F13/m2070_nooverlap_vcl!F33</f>
+        <v>1.5919142733081073</v>
       </c>
       <c r="U31" s="8">
-        <f>(m2070_nooverlap_vcl!G13-G13)/m2070_nooverlap_vcl!G13</f>
-        <v>0.77877914433155526</v>
+        <f>G13/m2070_nooverlap_vcl!G33</f>
+        <v>0.87794063095782393</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -7132,20 +7144,20 @@
         <v>4</v>
       </c>
       <c r="R32" s="8">
-        <f>(m2070_nooverlap_vcl!D14-D14)/m2070_nooverlap_vcl!D14</f>
-        <v>0.65770092258744695</v>
+        <f>D14/m2070_nooverlap_vcl!D34</f>
+        <v>3.8382693836796906</v>
       </c>
       <c r="S32" s="8">
-        <f>(m2070_nooverlap_vcl!E14-E14)/m2070_nooverlap_vcl!E14</f>
-        <v>0.53847549746618206</v>
+        <f>E14/m2070_nooverlap_vcl!E34</f>
+        <v>3.0993643509986084</v>
       </c>
       <c r="T32" s="8">
-        <f>(m2070_nooverlap_vcl!F14-F14)/m2070_nooverlap_vcl!F14</f>
-        <v>0.68427821468416117</v>
+        <f>F14/m2070_nooverlap_vcl!F34</f>
+        <v>2.193777435356</v>
       </c>
       <c r="U32" s="8">
-        <f>(m2070_nooverlap_vcl!G14-G14)/m2070_nooverlap_vcl!G14</f>
-        <v>0.71400542618132479</v>
+        <f>G14/m2070_nooverlap_vcl!G34</f>
+        <v>1.0793896490874773</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking off items from gordons list
</commit_message>
<xml_diff>
--- a/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
+++ b/latex/gpu_content/cascade_spmv/cascade_strong_scaling_benchmarks.xlsx
@@ -167,9 +167,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="440">
+  <cellStyleXfs count="444">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -622,7 +626,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="440">
+  <cellStyles count="444">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -842,6 +846,8 @@
     <cellStyle name="Followed Hyperlink" xfId="435" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="437" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="439" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1061,6 +1067,8 @@
     <cellStyle name="Hyperlink" xfId="434" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="436" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="438" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1309,12 +1317,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="2109991752"/>
-        <c:axId val="2062037704"/>
-        <c:axId val="2108617512"/>
+        <c:axId val="2126389304"/>
+        <c:axId val="2126396168"/>
+        <c:axId val="2126401656"/>
       </c:surfaceChart>
       <c:catAx>
-        <c:axId val="2109991752"/>
+        <c:axId val="2126389304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1342,7 +1350,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062037704"/>
+        <c:crossAx val="2126396168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1350,7 +1358,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2062037704"/>
+        <c:axId val="2126396168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -1380,13 +1388,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109991752"/>
+        <c:crossAx val="2126389304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2108617512"/>
+        <c:axId val="2126401656"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1422,7 +1430,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2062037704"/>
+        <c:crossAx val="2126396168"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -1717,12 +1725,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="2107691592"/>
-        <c:axId val="2107686072"/>
-        <c:axId val="2107680552"/>
+        <c:axId val="2126473720"/>
+        <c:axId val="2126479192"/>
+        <c:axId val="2126484680"/>
       </c:surfaceChart>
       <c:catAx>
-        <c:axId val="2107691592"/>
+        <c:axId val="2126473720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1758,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107686072"/>
+        <c:crossAx val="2126479192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1758,7 +1766,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2107686072"/>
+        <c:axId val="2126479192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -1788,13 +1796,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107691592"/>
+        <c:crossAx val="2126473720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2107680552"/>
+        <c:axId val="2126484680"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1830,7 +1838,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107686072"/>
+        <c:crossAx val="2126479192"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2125,12 +2133,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="2107641320"/>
-        <c:axId val="2110892168"/>
-        <c:axId val="2110897624"/>
+        <c:axId val="2125850200"/>
+        <c:axId val="2125844696"/>
+        <c:axId val="2125839176"/>
       </c:surfaceChart>
       <c:catAx>
-        <c:axId val="2107641320"/>
+        <c:axId val="2125850200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2158,7 +2166,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110892168"/>
+        <c:crossAx val="2125844696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2166,7 +2174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110892168"/>
+        <c:axId val="2125844696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -2196,13 +2204,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2107641320"/>
+        <c:crossAx val="2125850200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2110897624"/>
+        <c:axId val="2125839176"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2238,7 +2246,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110892168"/>
+        <c:crossAx val="2125844696"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -2533,12 +2541,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="2110936648"/>
-        <c:axId val="2110942152"/>
-        <c:axId val="2110947640"/>
+        <c:axId val="2125800072"/>
+        <c:axId val="2125794584"/>
+        <c:axId val="2125789096"/>
       </c:surfaceChart>
       <c:catAx>
-        <c:axId val="2110936648"/>
+        <c:axId val="2125800072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2566,7 +2574,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110942152"/>
+        <c:crossAx val="2125794584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2574,7 +2582,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2110942152"/>
+        <c:axId val="2125794584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="40.0"/>
@@ -2604,13 +2612,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110936648"/>
+        <c:crossAx val="2125800072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="8.0"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="2110947640"/>
+        <c:axId val="2125789096"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2646,7 +2654,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2110942152"/>
+        <c:crossAx val="2125794584"/>
         <c:crosses val="autoZero"/>
         <c:tickLblSkip val="1"/>
         <c:tickMarkSkip val="1"/>
@@ -3271,6 +3279,92 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="U3:Y9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="6">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="5">
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="1"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of GFLOP/s" fld="5" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
   <location ref="N3:R9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
@@ -3356,9 +3450,9 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable11" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="U3:Y9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="G3:K9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
@@ -3381,93 +3475,7 @@
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
         <item h="1" x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="1"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of GFLOP/s" fld="5" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium4" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="6">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
         <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
         <item t="default"/>
@@ -3529,8 +3537,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
-  <location ref="G3:K9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" gridDropZones="1" multipleFieldFilters="0">
+  <location ref="A3:E9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="6">
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
@@ -3552,8 +3560,8 @@
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="5">
-        <item h="1" x="0"/>
-        <item x="1"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
         <item h="1" x="2"/>
         <item h="1" x="3"/>
         <item t="default"/>
@@ -5163,8 +5171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T36" sqref="T36"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5396,7 +5404,7 @@
         <v>13.098146561096973</v>
       </c>
       <c r="N4" s="7">
-        <f t="shared" ref="N3:N14" si="3">(($B$1*G$2*2)/(G4*0.001))*0.000000001</f>
+        <f t="shared" ref="N4:N14" si="3">(($B$1*G$2*2)/(G4*0.001))*0.000000001</f>
         <v>13.457708003623891</v>
       </c>
       <c r="P4">
@@ -6499,17 +6507,14 @@
         <v>1</v>
       </c>
       <c r="S21" s="8">
-        <f t="shared" ref="S21:T21" si="5">E$3/(($C3)*E3)</f>
+        <f t="shared" ref="S21:U32" si="5">E$3/(($C3)*E3)</f>
         <v>1</v>
       </c>
       <c r="T21" s="8">
         <f t="shared" si="5"/>
         <v>1</v>
       </c>
-      <c r="U21" s="8" t="e">
-        <f>(N3/N$3)/C3</f>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="U21" s="8"/>
     </row>
     <row r="22" spans="1:23">
       <c r="A22">
@@ -6573,9 +6578,9 @@
         <f t="shared" si="7"/>
         <v>0.72430895764847347</v>
       </c>
-      <c r="U22" s="8" t="e">
-        <f t="shared" ref="U22:U32" si="8">(N4/N$3)/C4</f>
-        <v>#DIV/0!</v>
+      <c r="U22" s="8">
+        <f>G$4/(($C4/$C$4)*G4)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:23">
@@ -6607,42 +6612,42 @@
         <v>1</v>
       </c>
       <c r="K23" s="8">
-        <f t="shared" ref="K23:N23" si="9">D23/D5</f>
+        <f t="shared" ref="K23:N23" si="8">D23/D5</f>
         <v>0.91059306053177447</v>
       </c>
       <c r="L23" s="8">
+        <f t="shared" si="8"/>
+        <v>0.87459924797150201</v>
+      </c>
+      <c r="M23" s="8">
+        <f t="shared" si="8"/>
+        <v>0.90222366381951213</v>
+      </c>
+      <c r="N23" s="8">
+        <f t="shared" si="8"/>
+        <v>0.44682564129151892</v>
+      </c>
+      <c r="P23">
+        <v>4</v>
+      </c>
+      <c r="Q23">
+        <v>1</v>
+      </c>
+      <c r="R23" s="8">
+        <f t="shared" ref="R23:T23" si="9">D$3/(($C5)*D5)</f>
+        <v>0.38615170658118048</v>
+      </c>
+      <c r="S23" s="8">
         <f t="shared" si="9"/>
-        <v>0.87459924797150201</v>
-      </c>
-      <c r="M23" s="8">
+        <v>0.74950524440926181</v>
+      </c>
+      <c r="T23" s="8">
         <f t="shared" si="9"/>
-        <v>0.90222366381951213</v>
-      </c>
-      <c r="N23" s="8">
-        <f t="shared" si="9"/>
-        <v>0.44682564129151892</v>
-      </c>
-      <c r="P23">
-        <v>4</v>
-      </c>
-      <c r="Q23">
-        <v>1</v>
-      </c>
-      <c r="R23" s="8">
-        <f t="shared" ref="R23:T23" si="10">D$3/(($C5)*D5)</f>
-        <v>0.38615170658118048</v>
-      </c>
-      <c r="S23" s="8">
-        <f t="shared" si="10"/>
-        <v>0.74950524440926181</v>
-      </c>
-      <c r="T23" s="8">
-        <f t="shared" si="10"/>
         <v>0.68026273110606561</v>
       </c>
-      <c r="U23" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U23" s="8">
+        <f t="shared" ref="U23:U32" si="10">G$4/(($C5/$C$4)*G5)</f>
+        <v>0.93751467704403579</v>
       </c>
     </row>
     <row r="24" spans="1:23">
@@ -6707,9 +6712,9 @@
         <f t="shared" si="12"/>
         <v>0.56973917610517877</v>
       </c>
-      <c r="U24" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U24" s="8">
+        <f t="shared" si="10"/>
+        <v>0.99488164512308008</v>
       </c>
     </row>
     <row r="25" spans="1:23">
@@ -6774,9 +6779,9 @@
         <f t="shared" si="14"/>
         <v>0.66911562696633198</v>
       </c>
-      <c r="U25" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U25" s="8">
+        <f t="shared" si="10"/>
+        <v>0.9427648305409625</v>
       </c>
     </row>
     <row r="26" spans="1:23">
@@ -6841,9 +6846,9 @@
         <f t="shared" si="16"/>
         <v>0.63899060569300647</v>
       </c>
-      <c r="U26" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U26" s="8">
+        <f t="shared" si="10"/>
+        <v>0.91175476113502019</v>
       </c>
     </row>
     <row r="27" spans="1:23">
@@ -6908,9 +6913,9 @@
         <f t="shared" si="18"/>
         <v>0.6922767994679474</v>
       </c>
-      <c r="U27" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U27" s="8">
+        <f t="shared" si="10"/>
+        <v>0.99425739051685103</v>
       </c>
     </row>
     <row r="28" spans="1:23">
@@ -6975,9 +6980,9 @@
         <f t="shared" si="20"/>
         <v>0.41198303634569883</v>
       </c>
-      <c r="U28" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U28" s="8">
+        <f t="shared" si="10"/>
+        <v>0.81354245179156681</v>
       </c>
     </row>
     <row r="29" spans="1:23">
@@ -7042,9 +7047,9 @@
         <f t="shared" si="22"/>
         <v>0.77131561203849386</v>
       </c>
-      <c r="U29" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U29" s="8">
+        <f t="shared" si="10"/>
+        <v>0.90685678716612883</v>
       </c>
     </row>
     <row r="30" spans="1:23">
@@ -7109,9 +7114,9 @@
         <f t="shared" si="24"/>
         <v>0.51444281924558477</v>
       </c>
-      <c r="U30" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U30" s="8">
+        <f t="shared" si="10"/>
+        <v>0.94322477508990266</v>
       </c>
     </row>
     <row r="31" spans="1:23">
@@ -7176,9 +7181,9 @@
         <f t="shared" si="26"/>
         <v>0.39401638808134481</v>
       </c>
-      <c r="U31" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U31" s="8">
+        <f t="shared" si="10"/>
+        <v>0.75514518030853883</v>
       </c>
     </row>
     <row r="32" spans="1:23">
@@ -7243,9 +7248,9 @@
         <f t="shared" si="28"/>
         <v>0.30689533882964537</v>
       </c>
-      <c r="U32" s="8" t="e">
-        <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+      <c r="U32" s="8">
+        <f t="shared" si="10"/>
+        <v>0.60754086709872457</v>
       </c>
     </row>
     <row r="35" spans="15:21">

</xml_diff>